<commit_message>
Add todo list in source code
Last upload before leaving Japan
</commit_message>
<xml_diff>
--- a/Calibration Data/KENAF_Camera_Angle_Calibration.xlsx
+++ b/Calibration Data/KENAF_Camera_Angle_Calibration.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Work_Document\Y4\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tecnic08\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14923" windowHeight="6780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,11 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="187" formatCode="0.000"/>
-    <numFmt numFmtId="189" formatCode="0.00000"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,10 +81,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -107,7 +101,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -151,7 +145,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -314,7 +307,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$13</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -356,7 +349,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6A16-4FF4-8F34-3F92CF9D89A2}"/>
             </c:ext>
@@ -370,11 +363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1845718592"/>
-        <c:axId val="-1834142976"/>
+        <c:axId val="285822336"/>
+        <c:axId val="285818072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1845718592"/>
+        <c:axId val="285822336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,7 +413,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -487,12 +479,12 @@
             <a:endParaRPr lang="th-TH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1834142976"/>
+        <c:crossAx val="285818072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1834142976"/>
+        <c:axId val="285818072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -514,7 +506,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -544,7 +535,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -581,7 +572,7 @@
             <a:endParaRPr lang="th-TH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1845718592"/>
+        <c:crossAx val="285822336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -631,7 +622,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -675,7 +666,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -836,7 +826,7 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -878,7 +868,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CA5D-45EF-B5EA-F088755534E3}"/>
             </c:ext>
@@ -892,11 +882,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1834140800"/>
-        <c:axId val="-1834142432"/>
+        <c:axId val="646773904"/>
+        <c:axId val="646777512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1834140800"/>
+        <c:axId val="646773904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,7 +937,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1014,12 +1003,12 @@
             <a:endParaRPr lang="th-TH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1834142432"/>
+        <c:crossAx val="646777512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1834142432"/>
+        <c:axId val="646777512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1066,7 +1055,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1096,7 +1084,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1133,7 +1121,7 @@
             <a:endParaRPr lang="th-TH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1834140800"/>
+        <c:crossAx val="646773904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2298,16 +2286,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1360</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>17688</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>594632</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>58509</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2328,16 +2316,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>625248</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>78921</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304119</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>107496</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>461962</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2659,27 +2647,26 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.25" customWidth="1"/>
     <col min="9" max="9" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
@@ -2689,18 +2676,18 @@
         <v>38.810699999999997</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>241</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1.5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <f>ACOS($J3/B2)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <f>C2*360/(2*PI())</f>
         <v>0</v>
       </c>
@@ -2711,18 +2698,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>1.5009999999999999</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <f>ACOS($J3/B3)</f>
         <v>3.6504698516043099E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <f>C3*360/(2*PI())</f>
         <v>2.0915651573667491</v>
       </c>
@@ -2733,162 +2720,162 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>180</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>1.51</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <f>ACOS($J3/B4)</f>
         <v>0.11515067619063935</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <f t="shared" ref="D4:D13" si="0">C4*360/(2*PI())</f>
         <v>6.5976477538012102</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>160</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>1.5229999999999999</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <f>ACOS($J3/B5)</f>
         <v>0.17401113313911498</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>9.9701035171603447</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>140</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>1.542</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <f>ACOS($J3/B6)</f>
         <v>0.2339312107246363</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>13.403271070907161</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>120</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>1.5669999999999999</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <f>ACOS($J3/B7)</f>
         <v>0.2934793835416194</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>16.815130051035947</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>1.6</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <f>ACOS($J3/B8)</f>
         <v>0.3554212016902234</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>20.364134806317804</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>80</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>1.641</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <f>ACOS($J3/B9)</f>
         <v>0.41757078645661738</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>23.925043711922733</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>60</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>1.696</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <f>ACOS($J3/B10)</f>
         <v>0.4855166547877412</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>27.818055202647727</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>40</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>1.7569999999999999</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <f>ACOS($J3/B11)</f>
         <v>0.54769328113564009</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>31.380513476744245</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>1.835</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <f>ACOS($J3/B12)</f>
         <v>0.61384603634380019</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>35.170787153333897</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>1.925</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <f>ACOS($J3/B13)</f>
         <v>0.67737474526213792</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>38.810714052269759</v>
       </c>

</xml_diff>